<commit_message>
casos te teste de delete
</commit_message>
<xml_diff>
--- a/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
+++ b/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="1004">
   <si>
     <r>
       <t/>
@@ -23739,37 +23739,43 @@
     <t>Arquivo</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>GET</t>
   </si>
   <si>
     <t>cypress\e2e\api\validar_alergias_intolerancias.cy.js</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>cypress\e2e\api\validar_alimentos_da_guia.cy.js</t>
   </si>
   <si>
+    <t>api/alimentos-da-guia/</t>
+  </si>
+  <si>
     <t>POST</t>
   </si>
   <si>
+    <t>Fazendo</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
     <t>cypress\e2e\api\validar_alimentos.cy.js</t>
   </si>
   <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF1155cc"/>
-        <rFont val="monospace"/>
-        <family val="2"/>
-      </rPr>
-      <t>/api</t>
-    </r>
+    <t>/api/login</t>
   </si>
   <si>
     <t>cypress\e2e\api\validar_login.cy.js</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -24318,7 +24324,9 @@
       <c r="C1" s="9" t="s">
         <v>990</v>
       </c>
-      <c r="D1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>991</v>
+      </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -24344,12 +24352,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>992</v>
-      </c>
-      <c r="D2" s="10"/>
+        <v>993</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -24375,12 +24385,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>992</v>
-      </c>
-      <c r="D3" s="10"/>
+        <v>993</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -24406,12 +24418,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>993</v>
-      </c>
-      <c r="D4" s="10"/>
+        <v>995</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -24432,15 +24446,19 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="11" t="s">
-        <v>2</v>
+        <v>996</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>994</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="10"/>
+        <v>997</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>998</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -24466,12 +24484,14 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>993</v>
-      </c>
-      <c r="D6" s="10"/>
+        <v>995</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -24550,9 +24570,15 @@
       <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="13" t="s">
+        <v>999</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -24605,12 +24631,14 @@
         <v>5</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>995</v>
-      </c>
-      <c r="D11" s="10"/>
+        <v>1000</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -24636,12 +24664,14 @@
         <v>6</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>995</v>
-      </c>
-      <c r="D12" s="10"/>
+        <v>1000</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -42457,15 +42487,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="672" customHeight="1" ht="18.75">
       <c r="A672" s="15" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="B672" s="12" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>997</v>
-      </c>
-      <c r="D672" s="10"/>
+        <v>1002</v>
+      </c>
+      <c r="D672" s="10" t="s">
+        <v>1003</v>
+      </c>
       <c r="E672" s="10"/>
       <c r="F672" s="10"/>
       <c r="G672" s="10"/>

</xml_diff>

<commit_message>
caso de login sigpae
</commit_message>
<xml_diff>
--- a/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
+++ b/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="1007">
   <si>
     <r>
       <t/>
@@ -23760,10 +23760,19 @@
     <t>POST</t>
   </si>
   <si>
-    <t>Fazendo</t>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Patch</t>
   </si>
   <si>
     <t>DELETE</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
   <si>
     <t>cypress\e2e\api\validar_alimentos.cy.js</t>
@@ -24457,7 +24466,7 @@
         <v>995</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -24516,9 +24525,15 @@
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="13" t="s">
+        <v>998</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -24543,9 +24558,15 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="10"/>
+      <c r="B8" s="13" t="s">
+        <v>999</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -24570,8 +24591,8 @@
       <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>999</v>
+      <c r="B9" s="12" t="s">
+        <v>1000</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>995</v>
@@ -24603,9 +24624,15 @@
       <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>1002</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -24634,7 +24661,7 @@
         <v>992</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>994</v>
@@ -24667,7 +24694,7 @@
         <v>992</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>994</v>
@@ -42487,16 +42514,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="672" customHeight="1" ht="18.75">
       <c r="A672" s="15" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="B672" s="12" t="s">
         <v>997</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="D672" s="10" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="E672" s="10"/>
       <c r="F672" s="10"/>

</xml_diff>

<commit_message>
caso da rota alteracao cardapio
</commit_message>
<xml_diff>
--- a/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
+++ b/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="1008">
   <si>
     <r>
       <t/>
@@ -23776,6 +23776,9 @@
   </si>
   <si>
     <t>cypress\e2e\api\validar_alimentos.cy.js</t>
+  </si>
+  <si>
+    <t>cypress\e2e\api\validar_alteracoes_cardapio.cy.js</t>
   </si>
   <si>
     <t>/api/login</t>
@@ -24298,7 +24301,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="85.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="110.57642857142856" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="51.14785714285715" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -24525,7 +24528,7 @@
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>998</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -24558,7 +24561,7 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>999</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -24624,7 +24627,7 @@
       <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>1001</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -25911,9 +25914,15 @@
       <c r="A57" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="10"/>
+      <c r="B57" s="13" t="s">
+        <v>992</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
@@ -25938,7 +25947,9 @@
       <c r="A58" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="13"/>
+      <c r="B58" s="13" t="s">
+        <v>997</v>
+      </c>
       <c r="C58" s="12"/>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
@@ -25965,7 +25976,9 @@
       <c r="A59" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="13"/>
+      <c r="B59" s="13" t="s">
+        <v>992</v>
+      </c>
       <c r="C59" s="12"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
@@ -29336,7 +29349,7 @@
       <c r="V183" s="10"/>
       <c r="W183" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
       <c r="A184" s="11" t="s">
         <v>136</v>
       </c>
@@ -29363,7 +29376,7 @@
       <c r="V184" s="10"/>
       <c r="W184" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
       <c r="A185" s="11" t="s">
         <v>136</v>
       </c>
@@ -29390,7 +29403,7 @@
       <c r="V185" s="10"/>
       <c r="W185" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5">
       <c r="A186" s="11" t="s">
         <v>137</v>
       </c>
@@ -29417,7 +29430,7 @@
       <c r="V186" s="10"/>
       <c r="W186" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5">
       <c r="A187" s="11" t="s">
         <v>137</v>
       </c>
@@ -29444,7 +29457,7 @@
       <c r="V187" s="10"/>
       <c r="W187" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5">
       <c r="A188" s="11" t="s">
         <v>137</v>
       </c>
@@ -29471,7 +29484,7 @@
       <c r="V188" s="10"/>
       <c r="W188" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5">
       <c r="A189" s="11" t="s">
         <v>137</v>
       </c>
@@ -29498,7 +29511,7 @@
       <c r="V189" s="10"/>
       <c r="W189" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5">
       <c r="A190" s="11" t="s">
         <v>138</v>
       </c>
@@ -29525,7 +29538,7 @@
       <c r="V190" s="10"/>
       <c r="W190" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5">
       <c r="A191" s="11" t="s">
         <v>139</v>
       </c>
@@ -29552,7 +29565,7 @@
       <c r="V191" s="10"/>
       <c r="W191" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
       <c r="A192" s="11" t="s">
         <v>140</v>
       </c>
@@ -29579,7 +29592,7 @@
       <c r="V192" s="10"/>
       <c r="W192" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
       <c r="A193" s="11" t="s">
         <v>141</v>
       </c>
@@ -29606,7 +29619,7 @@
       <c r="V193" s="10"/>
       <c r="W193" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
       <c r="A194" s="11" t="s">
         <v>142</v>
       </c>
@@ -29633,7 +29646,7 @@
       <c r="V194" s="10"/>
       <c r="W194" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
       <c r="A195" s="11" t="s">
         <v>143</v>
       </c>
@@ -29660,7 +29673,7 @@
       <c r="V195" s="10"/>
       <c r="W195" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
       <c r="A196" s="11" t="s">
         <v>143</v>
       </c>
@@ -29687,7 +29700,7 @@
       <c r="V196" s="10"/>
       <c r="W196" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5">
       <c r="A197" s="11" t="s">
         <v>144</v>
       </c>
@@ -29714,7 +29727,7 @@
       <c r="V197" s="10"/>
       <c r="W197" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5">
       <c r="A198" s="11" t="s">
         <v>144</v>
       </c>
@@ -29741,7 +29754,7 @@
       <c r="V198" s="10"/>
       <c r="W198" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5">
       <c r="A199" s="11" t="s">
         <v>144</v>
       </c>
@@ -42514,16 +42527,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="672" customHeight="1" ht="18.75">
       <c r="A672" s="15" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B672" s="12" t="s">
         <v>997</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="D672" s="10" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E672" s="10"/>
       <c r="F672" s="10"/>

</xml_diff>

<commit_message>
casos de teste de alteraçoes cardapio
</commit_message>
<xml_diff>
--- a/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
+++ b/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="1008">
   <si>
     <r>
       <t/>
@@ -25914,7 +25914,7 @@
       <c r="A57" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="12" t="s">
         <v>992</v>
       </c>
       <c r="C57" s="12" t="s">
@@ -25947,7 +25947,7 @@
       <c r="A58" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>997</v>
       </c>
       <c r="C58" s="12"/>
@@ -25972,15 +25972,19 @@
       <c r="V58" s="10"/>
       <c r="W58" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="27">
       <c r="A59" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="10"/>
+      <c r="C59" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
@@ -26001,7 +26005,7 @@
       <c r="V59" s="10"/>
       <c r="W59" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="11" t="s">
         <v>45</v>
       </c>
@@ -26028,7 +26032,7 @@
       <c r="V60" s="10"/>
       <c r="W60" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="11" t="s">
         <v>45</v>
       </c>
@@ -26055,7 +26059,7 @@
       <c r="V61" s="10"/>
       <c r="W61" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="11" t="s">
         <v>45</v>
       </c>
@@ -26082,7 +26086,7 @@
       <c r="V62" s="10"/>
       <c r="W62" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="11" t="s">
         <v>45</v>
       </c>
@@ -26109,7 +26113,7 @@
       <c r="V63" s="10"/>
       <c r="W63" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
       <c r="A64" s="11" t="s">
         <v>46</v>
       </c>
@@ -26136,7 +26140,7 @@
       <c r="V64" s="10"/>
       <c r="W64" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="20.25">
       <c r="A65" s="11" t="s">
         <v>47</v>
       </c>
@@ -26163,7 +26167,7 @@
       <c r="V65" s="10"/>
       <c r="W65" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="20.25">
       <c r="A66" s="11" t="s">
         <v>48</v>
       </c>
@@ -26190,7 +26194,7 @@
       <c r="V66" s="10"/>
       <c r="W66" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="20.25">
       <c r="A67" s="11" t="s">
         <v>49</v>
       </c>
@@ -26217,7 +26221,7 @@
       <c r="V67" s="10"/>
       <c r="W67" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="20.25">
       <c r="A68" s="11" t="s">
         <v>50</v>
       </c>
@@ -26244,7 +26248,7 @@
       <c r="V68" s="10"/>
       <c r="W68" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="20.25">
       <c r="A69" s="11" t="s">
         <v>51</v>
       </c>
@@ -26271,7 +26275,7 @@
       <c r="V69" s="10"/>
       <c r="W69" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="20.25">
       <c r="A70" s="11" t="s">
         <v>52</v>
       </c>
@@ -26298,7 +26302,7 @@
       <c r="V70" s="10"/>
       <c r="W70" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="20.25">
       <c r="A71" s="11" t="s">
         <v>53</v>
       </c>
@@ -26325,13 +26329,19 @@
       <c r="V71" s="10"/>
       <c r="W71" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="20.25">
       <c r="A72" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="10"/>
+      <c r="B72" s="12" t="s">
+        <v>992</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
@@ -26352,7 +26362,7 @@
       <c r="V72" s="10"/>
       <c r="W72" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="20.25">
       <c r="A73" s="11" t="s">
         <v>55</v>
       </c>
@@ -26379,7 +26389,7 @@
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="20.25">
       <c r="A74" s="11" t="s">
         <v>56</v>
       </c>
@@ -26406,13 +26416,19 @@
       <c r="V74" s="10"/>
       <c r="W74" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="20.25">
       <c r="A75" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="10"/>
+      <c r="B75" s="12" t="s">
+        <v>992</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>994</v>
+      </c>
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
@@ -26433,11 +26449,13 @@
       <c r="V75" s="10"/>
       <c r="W75" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="20.25">
       <c r="A76" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B76" s="13"/>
+      <c r="B76" s="12" t="s">
+        <v>992</v>
+      </c>
       <c r="C76" s="12"/>
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
@@ -26460,11 +26478,13 @@
       <c r="V76" s="10"/>
       <c r="W76" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="20.25">
       <c r="A77" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B77" s="13"/>
+      <c r="B77" s="12" t="s">
+        <v>992</v>
+      </c>
       <c r="C77" s="12"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -26487,11 +26507,13 @@
       <c r="V77" s="10"/>
       <c r="W77" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="20.25">
       <c r="A78" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="12" t="s">
+        <v>992</v>
+      </c>
       <c r="C78" s="12"/>
       <c r="D78" s="10"/>
       <c r="E78" s="10"/>
@@ -26514,11 +26536,13 @@
       <c r="V78" s="10"/>
       <c r="W78" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="20.25">
       <c r="A79" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B79" s="13"/>
+      <c r="B79" s="12" t="s">
+        <v>992</v>
+      </c>
       <c r="C79" s="12"/>
       <c r="D79" s="10"/>
       <c r="E79" s="10"/>
@@ -26541,7 +26565,7 @@
       <c r="V79" s="10"/>
       <c r="W79" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="20.25">
       <c r="A80" s="11" t="s">
         <v>62</v>
       </c>
@@ -26568,7 +26592,7 @@
       <c r="V80" s="10"/>
       <c r="W80" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="20.25">
       <c r="A81" s="11" t="s">
         <v>63</v>
       </c>
@@ -26595,7 +26619,7 @@
       <c r="V81" s="10"/>
       <c r="W81" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="20.25">
       <c r="A82" s="11" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
casos de delete e metade dos cenarios de post da rota /api/alteracoes-cardapio/
</commit_message>
<xml_diff>
--- a/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
+++ b/cypress/fixtures/cenarios/Cobertura de Testes - SIGPAE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="1012">
   <si>
     <r>
       <t/>
@@ -23781,13 +23781,25 @@
     <t>cypress\e2e\api\validar_alteracoes_cardapio.cy.js</t>
   </si>
   <si>
+    <t>fazendo</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ver</t>
+  </si>
+  <si>
     <t>/api/login</t>
   </si>
   <si>
     <t>cypress\e2e\api\validar_login.cy.js</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -25613,7 +25625,7 @@
       <c r="V45" s="10"/>
       <c r="W45" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="11" t="s">
         <v>32</v>
       </c>
@@ -25640,7 +25652,7 @@
       <c r="V46" s="10"/>
       <c r="W46" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -25667,7 +25679,7 @@
       <c r="V47" s="10"/>
       <c r="W47" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="11" t="s">
         <v>34</v>
       </c>
@@ -25694,7 +25706,7 @@
       <c r="V48" s="10"/>
       <c r="W48" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="11" t="s">
         <v>35</v>
       </c>
@@ -25721,7 +25733,7 @@
       <c r="V49" s="10"/>
       <c r="W49" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="11" t="s">
         <v>36</v>
       </c>
@@ -25748,7 +25760,7 @@
       <c r="V50" s="10"/>
       <c r="W50" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
       <c r="A51" s="11" t="s">
         <v>37</v>
       </c>
@@ -25775,7 +25787,7 @@
       <c r="V51" s="10"/>
       <c r="W51" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="11" t="s">
         <v>38</v>
       </c>
@@ -25802,7 +25814,7 @@
       <c r="V52" s="10"/>
       <c r="W52" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="11" t="s">
         <v>39</v>
       </c>
@@ -25829,7 +25841,7 @@
       <c r="V53" s="10"/>
       <c r="W53" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
       <c r="A54" s="11" t="s">
         <v>40</v>
       </c>
@@ -25856,7 +25868,7 @@
       <c r="V54" s="10"/>
       <c r="W54" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
       <c r="A55" s="11" t="s">
         <v>41</v>
       </c>
@@ -25883,7 +25895,7 @@
       <c r="V55" s="10"/>
       <c r="W55" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
       <c r="A56" s="11" t="s">
         <v>42</v>
       </c>
@@ -25910,7 +25922,7 @@
       <c r="V56" s="10"/>
       <c r="W56" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
       <c r="A57" s="11" t="s">
         <v>43</v>
       </c>
@@ -25943,7 +25955,7 @@
       <c r="V57" s="10"/>
       <c r="W57" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="11" t="s">
         <v>43</v>
       </c>
@@ -25951,7 +25963,9 @@
         <v>997</v>
       </c>
       <c r="C58" s="12"/>
-      <c r="D58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>1005</v>
+      </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
@@ -26009,7 +26023,9 @@
       <c r="A60" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="13"/>
+      <c r="B60" s="12" t="s">
+        <v>1006</v>
+      </c>
       <c r="C60" s="12"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
@@ -26036,7 +26052,9 @@
       <c r="A61" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B61" s="13"/>
+      <c r="B61" s="12" t="s">
+        <v>1007</v>
+      </c>
       <c r="C61" s="12"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
@@ -26063,9 +26081,15 @@
       <c r="A62" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="10"/>
+      <c r="B62" s="12" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>1008</v>
+      </c>
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
@@ -26429,7 +26453,9 @@
       <c r="D75" s="10" t="s">
         <v>994</v>
       </c>
-      <c r="E75" s="10"/>
+      <c r="E75" s="10" t="s">
+        <v>1009</v>
+      </c>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
@@ -26456,9 +26482,15 @@
       <c r="B76" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
+      <c r="C76" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>1009</v>
+      </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
@@ -42551,16 +42583,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="672" customHeight="1" ht="18.75">
       <c r="A672" s="15" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="B672" s="12" t="s">
         <v>997</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="D672" s="10" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E672" s="10"/>
       <c r="F672" s="10"/>

</xml_diff>